<commit_message>
Auswertung Filter 2 fertig
</commit_message>
<xml_diff>
--- a/Messprotokoll.xlsx
+++ b/Messprotokoll.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
+    <sheet name="Diagramm2" sheetId="3" r:id="rId2"/>
+    <sheet name="Diagramm3" sheetId="4" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -197,7 +200,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Bode Diagramm 1</a:t>
+              <a:t>Bodediagramm 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -243,7 +246,505 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$Q$5:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>31.415926535897931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.831853071795862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125.66370614359172</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>251.32741228718345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376.99111843077515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>502.6548245743669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>628.31853071795865</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>753.98223686155029</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>942.47779607693792</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$P$5:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334019640"/>
+        <c:axId val="334022776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334019640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>omega</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334022776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="334022776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334019640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Bodediagramm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -301,41 +802,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$P$5:$P$13</c:f>
+              <c:f>Tabelle1!$O$5:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9</c:v>
+                  <c:v>-11.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6</c:v>
+                  <c:v>-51.43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>-127.74</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.03</c:v>
+                  <c:v>-144</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6</c:v>
+                  <c:v>-154.28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3</c:v>
+                  <c:v>-169.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -345,11 +846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="402419976"/>
-        <c:axId val="402419192"/>
+        <c:axId val="334021600"/>
+        <c:axId val="334024736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="402419976"/>
+        <c:axId val="334021600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -463,485 +964,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402419192"/>
+        <c:crossAx val="334024736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="402419192"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Amplitude</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="402419976"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Bodediagramm</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> 2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Tabelle1!$Q$5:$Q$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>31.415926535897931</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62.831853071795862</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>125.66370614359172</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>251.32741228718345</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>376.99111843077515</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>502.6548245743669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>628.31853071795865</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>753.98223686155029</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>942.47779607693792</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Tabelle1!$O$5:$O$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-11.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-51.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-127.74</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-144</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-154.28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-169.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="329580472"/>
-        <c:axId val="396372416"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="329580472"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Kreisfrequenz</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="396372416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="396372416"/>
+        <c:axId val="334024736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1082,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329580472"/>
+        <c:crossAx val="334021600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1095,11 +1123,356 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Nyquistdiagramm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$S$5:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47821033513633338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4226975775292621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.2106070141101959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89728182306331372</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.56525953745326873</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.29096804444263119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$R$5:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8388351952713966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.3069520109751172</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.1873341439723371</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50575224171542343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2012005350840716</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.305886060725969E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334018856"/>
+        <c:axId val="334019248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334018856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334019248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="334019248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334018856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -1183,6 +1556,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2215,25 +2628,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2246,24 +3200,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2271,12 +3222,39 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2545,8 +3523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,12 +3640,12 @@
         <v>31.415926535897931</v>
       </c>
       <c r="R5">
-        <f>-F5*SIN(O5*N5)</f>
+        <f>SIN(O5)*P5</f>
         <v>0</v>
       </c>
       <c r="S5">
-        <f>F5*COS(O5*N5)</f>
-        <v>0.13</v>
+        <f>P5*COS(O5)</f>
+        <v>1.3</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
@@ -2721,12 +3699,12 @@
         <v>62.831853071795862</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:R13" si="1">-F6*SIN(O6*N6)</f>
+        <f t="shared" ref="R6:R13" si="1">SIN(O6)*P6</f>
         <v>0</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:S13" si="2">F6*COS(O6*N6)</f>
-        <v>0.13</v>
+        <f t="shared" ref="S6:S13" si="2">P6*COS(O6)</f>
+        <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
@@ -2785,7 +3763,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="2"/>
-        <v>0.14000000000000001</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
@@ -2840,11 +3818,11 @@
       </c>
       <c r="R8">
         <f t="shared" si="1"/>
-        <v>7.830251219593376E-2</v>
+        <v>1.8388351952713966</v>
       </c>
       <c r="S8">
         <f t="shared" si="2"/>
-        <v>-0.17311474975808863</v>
+        <v>0.47821033513633338</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -2899,11 +3877,11 @@
       </c>
       <c r="R9">
         <f t="shared" si="1"/>
-        <v>-0.28419626901578338</v>
+        <v>-3.3069520109751172</v>
       </c>
       <c r="S9">
         <f t="shared" si="2"/>
-        <v>-0.22098072467414093</v>
+        <v>1.4226975775292621</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -2958,11 +3936,11 @@
       </c>
       <c r="R10">
         <f t="shared" si="1"/>
-        <v>7.1268826314763417E-2</v>
+        <v>-2.1873341439723371</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>-0.23962628068664774</v>
+        <v>-1.2106070141101959</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
@@ -3017,11 +3995,11 @@
       </c>
       <c r="R11">
         <f t="shared" si="1"/>
-        <v>-9.3025041741715622E-2</v>
+        <v>0.50575224171542343</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>-4.8696422958489118E-2</v>
+        <v>0.89728182306331372</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
@@ -3076,11 +4054,11 @@
       </c>
       <c r="R12">
         <f t="shared" si="1"/>
-        <v>3.6497176352058666E-2</v>
+        <v>0.2012005350840716</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
-        <v>-4.7623062882669875E-2</v>
+        <v>-0.56525953745326873</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
@@ -3135,15 +4113,14 @@
       </c>
       <c r="R13">
         <f t="shared" si="1"/>
-        <v>2.9639107095575351E-2</v>
+        <v>7.305886060725969E-2</v>
       </c>
       <c r="S13">
         <f t="shared" si="2"/>
-        <v>-4.6393243664368776E-3</v>
+        <v>0.29096804444263119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Achsenbeschriftung der Graphen ergänzt und Bilder größer gemacht
</commit_message>
<xml_diff>
--- a/Messprotokoll.xlsx
+++ b/Messprotokoll.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
@@ -378,11 +378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334019640"/>
-        <c:axId val="334022776"/>
+        <c:axId val="-1324782272"/>
+        <c:axId val="-1324770304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334019640"/>
+        <c:axId val="-1324782272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,8 +423,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>omega</a:t>
+                  <a:t>Kreisfrequenz</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -495,13 +500,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334022776"/>
+        <c:crossAx val="-1324770304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334022776"/>
+        <c:axId val="-1324770304"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -541,7 +547,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Amplitude</a:t>
+                  <a:t>Amplitudenverhältnis</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -613,7 +619,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334019640"/>
+        <c:crossAx val="-1324782272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -846,11 +852,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334021600"/>
-        <c:axId val="334024736"/>
+        <c:axId val="-1324771936"/>
+        <c:axId val="-1324771392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334021600"/>
+        <c:axId val="-1324771936"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -892,8 +898,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>omega</a:t>
+                  <a:t>Kreisfrequenz</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -964,12 +975,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334024736"/>
+        <c:crossAx val="-1324771392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334024736"/>
+        <c:axId val="-1324771392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1021,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Phasenverschiebung</a:t>
+                  <a:t>Phasenverschiebung [°]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1082,7 +1093,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334021600"/>
+        <c:crossAx val="-1324771936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1309,11 +1320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334018856"/>
-        <c:axId val="334019248"/>
+        <c:axId val="-1140922016"/>
+        <c:axId val="-1140923104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334018856"/>
+        <c:axId val="-1140922016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,6 +1344,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Realteil</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1370,12 +1437,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334019248"/>
+        <c:crossAx val="-1140923104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334019248"/>
+        <c:axId val="-1140923104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,6 +1462,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Imaginärteil</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.5600145776780221E-3"/>
+              <c:y val="0.4557688480474868"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1432,7 +1562,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334018856"/>
+        <c:crossAx val="-1140922016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3148,7 +3278,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3159,7 +3289,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3170,7 +3300,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3181,7 +3311,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304020" cy="6019800"/>
+    <xdr:ext cx="9299149" cy="6009588"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3208,7 +3338,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304020" cy="6019800"/>
+    <xdr:ext cx="9299149" cy="6009588"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3235,7 +3365,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304020" cy="6019800"/>
+    <xdr:ext cx="9299149" cy="6009588"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3523,7 +3653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Satz zum Diagramm entfernt und in Excel Achse auf logarithmisch gestellt
</commit_message>
<xml_diff>
--- a/Messprotokoll.xlsx
+++ b/Messprotokoll.xlsx
@@ -378,12 +378,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324782272"/>
-        <c:axId val="-1324770304"/>
+        <c:axId val="326230328"/>
+        <c:axId val="326227584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324782272"/>
+        <c:axId val="326230328"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -500,12 +501,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324770304"/>
+        <c:crossAx val="326227584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324770304"/>
+        <c:axId val="326227584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -619,7 +620,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324782272"/>
+        <c:crossAx val="326230328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -852,11 +853,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324771936"/>
-        <c:axId val="-1324771392"/>
+        <c:axId val="325795648"/>
+        <c:axId val="325801136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324771936"/>
+        <c:axId val="325795648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -975,12 +976,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324771392"/>
+        <c:crossAx val="325801136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324771392"/>
+        <c:axId val="325801136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1094,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324771936"/>
+        <c:crossAx val="325795648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1320,11 +1321,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1140922016"/>
-        <c:axId val="-1140923104"/>
+        <c:axId val="325799176"/>
+        <c:axId val="325796824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1140922016"/>
+        <c:axId val="325799176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,12 +1438,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1140923104"/>
+        <c:crossAx val="325796824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1140923104"/>
+        <c:axId val="325796824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,7 +1563,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1140922016"/>
+        <c:crossAx val="325799176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3278,7 +3279,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3289,7 +3290,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3300,7 +3301,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3311,7 +3312,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9299149" cy="6009588"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3338,7 +3339,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9299149" cy="6009588"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3365,7 +3366,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9299149" cy="6009588"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>

</xml_diff>